<commit_message>
Review and fix some bugs in system feature sheet
</commit_message>
<xml_diff>
--- a/Requirement Management/Software Requirement Specification/[HRM]Funtional Requirement and Business Rule.xlsx
+++ b/Requirement Management/Software Requirement Specification/[HRM]Funtional Requirement and Business Rule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="17400" windowHeight="8505"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="17400" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Funtional Requirements" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>Assessment Management</t>
   </si>
   <si>
-    <t>Attendance Tracking Management</t>
-  </si>
-  <si>
     <t>Personal Information Management</t>
   </si>
   <si>
@@ -379,9 +376,6 @@
   </si>
   <si>
     <t>Priority</t>
-  </si>
-  <si>
-    <t>Manage HRM system; include user management, authentication, configuration, etc. This feature will be hidden and filtered by users'</t>
   </si>
   <si>
     <t>High</t>
@@ -548,6 +542,12 @@
   </si>
   <si>
     <t>UC.PIM.3.3</t>
+  </si>
+  <si>
+    <t>Employee Labor Management</t>
+  </si>
+  <si>
+    <t>Manage HRM system; include user management, authentication, configuration, etc. This feature will be hidden and filtered by users' permission</t>
   </si>
 </sst>
 </file>
@@ -821,6 +821,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -833,44 +857,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
@@ -1178,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,27 +1193,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1229,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1237,16 +1237,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1254,16 +1254,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1271,16 +1271,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1288,16 +1288,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1305,16 +1305,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1322,16 +1322,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1339,16 +1339,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1356,16 +1356,16 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1373,16 +1373,16 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1390,16 +1390,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1407,16 +1407,16 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1424,16 +1424,16 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1441,16 +1441,16 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1458,16 +1458,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1475,16 +1475,16 @@
         <v>15</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1492,16 +1492,16 @@
         <v>16</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1518,7 +1518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1532,199 +1532,199 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>79</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>77</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>46</v>
+      <c r="B14" s="33" t="s">
+        <v>45</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1754,24 +1754,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1781,10 +1781,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1792,13 +1792,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1806,13 +1806,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1820,13 +1820,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1834,13 +1834,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1848,13 +1848,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1862,13 +1862,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1876,13 +1876,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1890,13 +1890,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1904,13 +1904,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1918,13 +1918,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1932,13 +1932,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1946,13 +1946,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1960,13 +1960,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1974,13 +1974,13 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1988,13 +1988,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2002,13 +2002,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2016,13 +2016,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2030,13 +2030,13 @@
         <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2044,13 +2044,13 @@
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2058,13 +2058,13 @@
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2108,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,143 +2122,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="28" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="31" t="s">
+    <row r="4" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="34" t="s">
+    <row r="5" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="C5" s="27" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="30" t="s">
+      <c r="D5" s="27" t="s">
         <v>117</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>119</v>
+      <c r="C6" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
     </row>
-    <row r="8" spans="1:4" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
+    <row r="8" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="34" t="s">
+      <c r="D10" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="34" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="31" t="s">
+      <c r="D11" s="30" t="s">
         <v>123</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manage Document - Curriculum  fixed: Manage Cirriculum Manage Project - Research  fixed: Manage Project Manage probation progress fixed: Manage Probation Manage Task fixed: Manage Working Progress Manage Wage Change fixed Manage Wage Progress Penalty fixed: discipline Equipment fixed Facilitate
</commit_message>
<xml_diff>
--- a/Requirement Management/Software Requirement Specification/[HRM]Funtional Requirement and Business Rule.xlsx
+++ b/Requirement Management/Software Requirement Specification/[HRM]Funtional Requirement and Business Rule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="17400" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="17400" windowHeight="8385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Funtional Requirements" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Funtional Requirements'!$A$4:$C$4</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="185">
   <si>
     <t>Description</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Manage position</t>
   </si>
   <si>
-    <t>Manage profile</t>
-  </si>
-  <si>
     <t>Manage family relationship</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>Manage wage progress</t>
   </si>
   <si>
-    <t>Manage reward &amp; penalty</t>
-  </si>
-  <si>
     <t>Manage Facilitate</t>
   </si>
   <si>
@@ -171,9 +165,6 @@
   </si>
   <si>
     <t>Allow the HRM staff to keep track of changing in wage of the staff at the Van Lang University</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allow the HRM staff to record the process of reward or penalty of the staff </t>
   </si>
   <si>
     <t xml:space="preserve">Allow the HRM staff to record the providing the facilitates for the staff </t>
@@ -214,9 +205,6 @@
  update it in system</t>
   </si>
   <si>
-    <t>Functional</t>
-  </si>
-  <si>
     <t>Allow the HRM staff create new information about staff/lecture
 HRM system allows user to import personal information from excel file, helps users to transfer all their current data (excel files) to proposed system's data
 HRM system allows user to export employee information following users' defined conditions into excel or doc</t>
@@ -233,11 +221,6 @@
   </si>
   <si>
     <t>BR3</t>
-  </si>
-  <si>
-    <t>Create new HR
- + Import personal information
- +Export information</t>
   </si>
   <si>
     <t xml:space="preserve">General (log in 
@@ -262,17 +245,10 @@
     <t>System must  supply add,edit catalog for user</t>
   </si>
   <si>
-    <t>General (Change)</t>
-  </si>
-  <si>
     <t>When HRD staff update and fix information (detail information,
  extend information, profile….) must be logged.</t>
   </si>
   <si>
-    <t>Manage reward 
-&amp; penalty</t>
-  </si>
-  <si>
     <t>Assessment management do once a year, and HRD staff 
 must update information about reward.</t>
   </si>
@@ -316,9 +292,6 @@
   </si>
   <si>
     <t>Tung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manage Project - Research </t>
   </si>
   <si>
     <t>Manage Profile</t>
@@ -548,6 +521,106 @@
   </si>
   <si>
     <t>Manage HRM system; include user management, authentication, configuration, etc. This feature will be hidden and filtered by users' permission</t>
+  </si>
+  <si>
+    <t>Ghi lại các giấy tờ quyết định, scan,…Ví dụ như tuyển dụng thành công thì có giấy tờ xác nhận hoặc mục check xác nhận</t>
+  </si>
+  <si>
+    <t>Nhân viên cần có chứng chỉ: giáo sư, phó giáo sư</t>
+  </si>
+  <si>
+    <t>Quản lý trang thiết bị: ghi lại thời gian sử dụng thiết bị và các giấy tờ sử dụng, giấy tờ cho mượn (hệ thống ghi nhận lại các giấy tờ đó như thế nào?)</t>
+  </si>
+  <si>
+    <t>Quản lý đào tạo: cập nhật thông tin bằng cấp, sau đó dựa vào đó để xét lương</t>
+  </si>
+  <si>
+    <t>Ngoài file excel còn file nào khác?</t>
+  </si>
+  <si>
+    <t>Báo cáo: hạn hợp đồng, TG1, TG2, hạn sử dụng trang thiết bị???</t>
+  </si>
+  <si>
+    <t>Manage facilitate</t>
+  </si>
+  <si>
+    <t>Manage reward 
+&amp; manage discipline</t>
+  </si>
+  <si>
+    <t>General (change)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manage Science Research </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create new information is not empty value </t>
+  </si>
+  <si>
+    <t>Quản lý khen thưởng và kỉ luật: xử lí thông tin 1 năm thì cập nhật vào ql đánh giá. Hỏi cần phần mềm làm sao chỗ này</t>
+  </si>
+  <si>
+    <t>Functional concerned</t>
+  </si>
+  <si>
+    <t>Create new HR
+ + Import personal information
+ + Export information</t>
+  </si>
+  <si>
+    <t>Manage working progress</t>
+  </si>
+  <si>
+    <t>FR.PIM.2.12</t>
+  </si>
+  <si>
+    <t>FR.PIM.2.13</t>
+  </si>
+  <si>
+    <t>FR.PIM.2.14</t>
+  </si>
+  <si>
+    <t>FR.PIM.2.15</t>
+  </si>
+  <si>
+    <t>Allow the HRM staff to manage Army Rank information</t>
+  </si>
+  <si>
+    <t>Allow the HRM staff to manage Union Task information</t>
+  </si>
+  <si>
+    <t>Allow the HRM staff to manage Labor Union information</t>
+  </si>
+  <si>
+    <t>Allow the HRM staff to manage Communist Party Task information</t>
+  </si>
+  <si>
+    <t>Nhung Huynh</t>
+  </si>
+  <si>
+    <t>Manage army rank</t>
+  </si>
+  <si>
+    <t>Manage labor union</t>
+  </si>
+  <si>
+    <t>Manage union task</t>
+  </si>
+  <si>
+    <t>Manage communist party task</t>
+  </si>
+  <si>
+    <t>Manage profile
++ Manage project
++ Manage curriculum
++ Manage article
++ Manage thesis guidance</t>
+  </si>
+  <si>
+    <t>Manage reward and discipline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allow the HRM staff to record the process of reward or discipline of the staff </t>
   </si>
 </sst>
 </file>
@@ -627,7 +700,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,6 +722,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3DFEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -788,9 +867,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -845,15 +921,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -874,6 +961,19 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1176,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,27 +1293,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1237,13 +1337,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>27</v>
@@ -1254,13 +1354,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>27</v>
@@ -1271,13 +1371,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>27</v>
@@ -1288,13 +1388,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>27</v>
@@ -1305,13 +1405,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>168</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>27</v>
@@ -1322,13 +1422,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>27</v>
@@ -1339,13 +1439,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>27</v>
@@ -1356,13 +1456,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>42</v>
+        <v>183</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>50</v>
+        <v>184</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>27</v>
@@ -1373,30 +1473,30 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>52</v>
+        <v>125</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>49</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>27</v>
@@ -1407,13 +1507,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>27</v>
@@ -1424,13 +1524,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>27</v>
@@ -1441,66 +1541,134 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>63</v>
+        <v>169</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="E18" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>18</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>15</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="C19" s="11" t="s">
+    <row r="23" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>19</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>16</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C20" s="13" t="s">
+    <row r="24" spans="1:5" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>20</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D24" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1516,185 +1684,200 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="14" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>36</v>
+        <v>60</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>74</v>
+      <c r="C7" s="18" t="s">
+        <v>69</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:5" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="33" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E8" s="34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>76</v>
+      <c r="B12" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>65</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>45</v>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>43</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>23</v>
@@ -1702,36 +1885,52 @@
       <c r="D14" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="7" t="s">
-        <v>24</v>
+      <c r="E14" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="35" t="s">
+        <v>164</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>19</v>
-      </c>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:D3"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1742,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,24 +1953,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1792,13 +1991,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1806,13 +2005,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1820,13 +2019,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1834,13 +2033,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1848,13 +2047,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1862,13 +2061,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1876,13 +2075,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1890,13 +2089,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1904,13 +2103,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1918,13 +2117,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1932,13 +2131,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>92</v>
+        <v>163</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1946,13 +2145,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1960,13 +2159,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1974,13 +2173,13 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1988,13 +2187,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2002,13 +2201,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2016,13 +2215,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2030,13 +2229,13 @@
         <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2044,13 +2243,13 @@
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2058,13 +2257,13 @@
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2108,8 +2307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,143 +2321,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="24" t="s">
+      <c r="D6" s="43" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="40"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+    </row>
+    <row r="8" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="D3" s="27" t="s">
+      <c r="D8" s="26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="30" t="s">
+      <c r="D9" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D10" s="26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="26" t="s">
+      <c r="D11" s="29" t="s">
         <v>115</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-    </row>
-    <row r="8" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>